<commit_message>
avance II a arquitectura de software
</commit_message>
<xml_diff>
--- a/SILESWEB/DOCUMENTACION/Graficos Arquitectura.xlsx
+++ b/SILESWEB/DOCUMENTACION/Graficos Arquitectura.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\SILESWEB\SILESWEB\DOCUMENTACION\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fredy Sarmiento\Documents\SilesWeb\SILESWEB\DOCUMENTACION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0558A189-AC9D-4E98-A642-EB673BC808D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5422D35C-91BA-4492-8647-44853759A004}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -62,12 +61,6 @@
     <t>Flujos de Negocio</t>
   </si>
   <si>
-    <t>Compnente de Negocio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Entidad de Negocios </t>
-  </si>
-  <si>
     <t>Seguridad</t>
   </si>
   <si>
@@ -88,11 +81,17 @@
   <si>
     <t>Componentes de Acceso a Datos</t>
   </si>
+  <si>
+    <t>Componente de Negocio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entidades de Negocios </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -676,33 +675,6 @@
   </cellStyleXfs>
   <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
@@ -726,60 +698,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="39" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="40" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="41" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="42" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -789,6 +713,42 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="44" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -816,15 +776,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
@@ -834,8 +785,56 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -874,7 +873,7 @@
         <xdr:cNvPr id="3" name="Gráfico 2" descr="Usuario con relleno sólido">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D5699CD-6EA2-0A4B-9BE8-D9C738F2B1A9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7D5699CD-6EA2-0A4B-9BE8-D9C738F2B1A9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -883,13 +882,13 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
             <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
-              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" xmlns="" r:embed="rId2"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -917,8 +916,8 @@
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>838200</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
@@ -927,7 +926,7 @@
         <xdr:cNvPr id="7" name="Gráfico 6" descr="Cubo con relleno sólido">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0FB1C48-9484-351F-8D5D-CB4189CAEBF9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D0FB1C48-9484-351F-8D5D-CB4189CAEBF9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -936,13 +935,13 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
             <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
-              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId4"/>
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" xmlns="" r:embed="rId4"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -980,7 +979,7 @@
         <xdr:cNvPr id="9" name="Gráfico 8" descr="Cilindro con relleno sólido">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1456B646-C12E-0967-76E8-AE138FC10996}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1456B646-C12E-0967-76E8-AE138FC10996}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -989,13 +988,13 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
             <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
-              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId6"/>
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" xmlns="" r:embed="rId6"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1033,7 +1032,7 @@
         <xdr:cNvPr id="11" name="Conector recto de flecha 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D669E2C8-0FAD-4E56-1CB3-83AA42571175}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D669E2C8-0FAD-4E56-1CB3-83AA42571175}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1086,7 +1085,7 @@
         <xdr:cNvPr id="12" name="Conector recto de flecha 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82761898-B833-467C-A2CE-0A039BCD20FC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{82761898-B833-467C-A2CE-0A039BCD20FC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1139,7 +1138,7 @@
         <xdr:cNvPr id="15" name="Conector recto de flecha 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1AC8E94-ED94-4B9B-929D-0ABE69388898}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B1AC8E94-ED94-4B9B-929D-0ABE69388898}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1153,7 +1152,7 @@
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln w="38100">
+        <a:ln>
           <a:tailEnd type="triangle"/>
         </a:ln>
       </xdr:spPr>
@@ -1192,7 +1191,7 @@
         <xdr:cNvPr id="18" name="Conector recto de flecha 17">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42D3428D-55E9-B472-2EEE-40F486303447}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{42D3428D-55E9-B472-2EEE-40F486303447}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1206,7 +1205,7 @@
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln w="19050">
+        <a:ln>
           <a:headEnd type="triangle"/>
           <a:tailEnd type="triangle"/>
         </a:ln>
@@ -1246,7 +1245,7 @@
         <xdr:cNvPr id="22" name="Conector recto de flecha 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{118F83BF-475A-4214-A280-4EC72A30B28C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{118F83BF-475A-4214-A280-4EC72A30B28C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1581,535 +1580,527 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7E4D475-9637-4F9B-B553-E02103C210E8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V22" sqref="V22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9:N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" style="20" customWidth="1"/>
+    <col min="1" max="1" width="8.5703125" style="11" customWidth="1"/>
     <col min="2" max="2" width="2.5703125" customWidth="1"/>
     <col min="4" max="4" width="2" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
     <col min="6" max="6" width="1.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
     <col min="8" max="8" width="2.28515625" customWidth="1"/>
-    <col min="9" max="9" width="2.5703125" style="20" customWidth="1"/>
+    <col min="9" max="9" width="2.5703125" style="11" customWidth="1"/>
     <col min="10" max="10" width="5.28515625" customWidth="1"/>
-    <col min="11" max="11" width="1.85546875" style="20" customWidth="1"/>
+    <col min="11" max="11" width="1.85546875" style="11" customWidth="1"/>
     <col min="12" max="12" width="5.85546875" customWidth="1"/>
-    <col min="13" max="13" width="1.85546875" style="20" customWidth="1"/>
+    <col min="13" max="13" width="1.85546875" style="11" customWidth="1"/>
     <col min="14" max="14" width="5.7109375" customWidth="1"/>
-    <col min="15" max="15" width="3.140625" style="20" customWidth="1"/>
+    <col min="15" max="15" width="3.140625" style="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="N1" s="20"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="N1" s="11"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="N2" s="20"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="N2" s="11"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B3" s="34"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="N3" s="20"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="N3" s="11"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="34"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="20"/>
-      <c r="L4" s="20"/>
-      <c r="N4" s="20"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="62"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="N4" s="11"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="34"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="20"/>
-      <c r="L5" s="20"/>
-      <c r="N5" s="20"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="61"/>
+      <c r="H5" s="62"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="N5" s="11"/>
     </row>
     <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="36"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="20"/>
-      <c r="L6" s="20"/>
-      <c r="N6" s="20"/>
-    </row>
-    <row r="7" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:14" s="20" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+      <c r="B6" s="63"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="64"/>
+      <c r="H6" s="65"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="N6" s="11"/>
+    </row>
+    <row r="7" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:14" s="11" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:14" ht="6.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="70" t="s">
+      <c r="A9" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="24"/>
-      <c r="J9" s="67" t="s">
+      <c r="B9" s="13"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="15"/>
+      <c r="J9" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="K9" s="33"/>
+      <c r="L9" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="M9" s="33"/>
+      <c r="N9" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="K9" s="73"/>
-      <c r="L9" s="67" t="s">
+    </row>
+    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="54"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="66" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="67"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="67"/>
+      <c r="G10" s="68"/>
+      <c r="H10" s="17"/>
+      <c r="J10" s="35"/>
+      <c r="K10" s="33"/>
+      <c r="L10" s="35"/>
+      <c r="M10" s="33"/>
+      <c r="N10" s="35"/>
+    </row>
+    <row r="11" spans="1:14" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="54"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="17"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="33"/>
+      <c r="L11" s="35"/>
+      <c r="M11" s="33"/>
+      <c r="N11" s="35"/>
+    </row>
+    <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="54"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="66" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="67"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="67"/>
+      <c r="G12" s="68"/>
+      <c r="H12" s="17"/>
+      <c r="J12" s="35"/>
+      <c r="K12" s="33"/>
+      <c r="L12" s="35"/>
+      <c r="M12" s="33"/>
+      <c r="N12" s="35"/>
+    </row>
+    <row r="13" spans="1:14" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="54"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="21"/>
+      <c r="J13" s="35"/>
+      <c r="K13" s="33"/>
+      <c r="L13" s="35"/>
+      <c r="M13" s="33"/>
+      <c r="N13" s="35"/>
+    </row>
+    <row r="14" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="J14" s="35"/>
+      <c r="K14" s="33"/>
+      <c r="L14" s="35"/>
+      <c r="M14" s="33"/>
+      <c r="N14" s="35"/>
+    </row>
+    <row r="15" spans="1:14" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="35"/>
+      <c r="K15" s="33"/>
+      <c r="L15" s="35"/>
+      <c r="M15" s="33"/>
+      <c r="N15" s="35"/>
+    </row>
+    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="55"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="69" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="70"/>
+      <c r="E16" s="70"/>
+      <c r="F16" s="70"/>
+      <c r="G16" s="71"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="35"/>
+      <c r="K16" s="33"/>
+      <c r="L16" s="35"/>
+      <c r="M16" s="33"/>
+      <c r="N16" s="35"/>
+    </row>
+    <row r="17" spans="1:14" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="55"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="35"/>
+      <c r="K17" s="33"/>
+      <c r="L17" s="35"/>
+      <c r="M17" s="33"/>
+      <c r="N17" s="35"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="55"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="72" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="6"/>
+      <c r="E18" s="72" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="6"/>
+      <c r="G18" s="72" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" s="5"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="35"/>
+      <c r="K18" s="33"/>
+      <c r="L18" s="35"/>
+      <c r="M18" s="33"/>
+      <c r="N18" s="35"/>
+    </row>
+    <row r="19" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="55"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="73"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="73"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="73"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="35"/>
+      <c r="K19" s="33"/>
+      <c r="L19" s="35"/>
+      <c r="M19" s="33"/>
+      <c r="N19" s="35"/>
+    </row>
+    <row r="20" spans="1:14" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="55"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="35"/>
+      <c r="K20" s="33"/>
+      <c r="L20" s="35"/>
+      <c r="M20" s="33"/>
+      <c r="N20" s="35"/>
+    </row>
+    <row r="21" spans="1:14" s="11" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="35"/>
+      <c r="K21" s="33"/>
+      <c r="L21" s="35"/>
+      <c r="M21" s="33"/>
+      <c r="N21" s="35"/>
+    </row>
+    <row r="22" spans="1:14" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="56" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="22"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="35"/>
+      <c r="K22" s="33"/>
+      <c r="L22" s="35"/>
+      <c r="M22" s="33"/>
+      <c r="N22" s="35"/>
+    </row>
+    <row r="23" spans="1:14" ht="22.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="56"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="38"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="M9" s="73"/>
-      <c r="N9" s="67" t="s">
+      <c r="G23" s="42"/>
+      <c r="H23" s="27"/>
+      <c r="J23" s="35"/>
+      <c r="K23" s="33"/>
+      <c r="L23" s="35"/>
+      <c r="M23" s="33"/>
+      <c r="N23" s="35"/>
+    </row>
+    <row r="24" spans="1:14" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="56"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="44"/>
+      <c r="H24" s="27"/>
+      <c r="J24" s="35"/>
+      <c r="K24" s="33"/>
+      <c r="L24" s="35"/>
+      <c r="M24" s="33"/>
+      <c r="N24" s="35"/>
+    </row>
+    <row r="25" spans="1:14" ht="9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="56"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="32"/>
+      <c r="J25" s="36"/>
+      <c r="K25" s="33"/>
+      <c r="L25" s="36"/>
+      <c r="M25" s="33"/>
+      <c r="N25" s="36"/>
+    </row>
+    <row r="26" spans="1:14" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="L26" s="11"/>
+      <c r="N26" s="11"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B27" s="45" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="70"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="26"/>
-      <c r="J10" s="68"/>
-      <c r="K10" s="73"/>
-      <c r="L10" s="68"/>
-      <c r="M10" s="73"/>
-      <c r="N10" s="68"/>
-    </row>
-    <row r="11" spans="1:14" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="70"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="26"/>
-      <c r="J11" s="68"/>
-      <c r="K11" s="73"/>
-      <c r="L11" s="68"/>
-      <c r="M11" s="73"/>
-      <c r="N11" s="68"/>
-    </row>
-    <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="70"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="26"/>
-      <c r="J12" s="68"/>
-      <c r="K12" s="73"/>
-      <c r="L12" s="68"/>
-      <c r="M12" s="73"/>
-      <c r="N12" s="68"/>
-    </row>
-    <row r="13" spans="1:14" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="70"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="30"/>
-      <c r="J13" s="68"/>
-      <c r="K13" s="73"/>
-      <c r="L13" s="68"/>
-      <c r="M13" s="73"/>
-      <c r="N13" s="68"/>
-    </row>
-    <row r="14" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="J14" s="68"/>
-      <c r="K14" s="73"/>
-      <c r="L14" s="68"/>
-      <c r="M14" s="73"/>
-      <c r="N14" s="68"/>
-    </row>
-    <row r="15" spans="1:14" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="71" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="68"/>
-      <c r="K15" s="73"/>
-      <c r="L15" s="68"/>
-      <c r="M15" s="73"/>
-      <c r="N15" s="68"/>
-    </row>
-    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="71"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="68"/>
-      <c r="K16" s="73"/>
-      <c r="L16" s="68"/>
-      <c r="M16" s="73"/>
-      <c r="N16" s="68"/>
-    </row>
-    <row r="17" spans="1:14" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="71"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="68"/>
-      <c r="K17" s="73"/>
-      <c r="L17" s="68"/>
-      <c r="M17" s="73"/>
-      <c r="N17" s="68"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="71"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" s="15"/>
-      <c r="E18" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="F18" s="15"/>
-      <c r="G18" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H18" s="14"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="68"/>
-      <c r="K18" s="73"/>
-      <c r="L18" s="68"/>
-      <c r="M18" s="73"/>
-      <c r="N18" s="68"/>
-    </row>
-    <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="71"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="68"/>
-      <c r="K19" s="73"/>
-      <c r="L19" s="68"/>
-      <c r="M19" s="73"/>
-      <c r="N19" s="68"/>
-    </row>
-    <row r="20" spans="1:14" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="71"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="68"/>
-      <c r="K20" s="73"/>
-      <c r="L20" s="68"/>
-      <c r="M20" s="73"/>
-      <c r="N20" s="68"/>
-    </row>
-    <row r="21" spans="1:14" s="20" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="19"/>
-      <c r="J21" s="68"/>
-      <c r="K21" s="73"/>
-      <c r="L21" s="68"/>
-      <c r="M21" s="73"/>
-      <c r="N21" s="68"/>
-    </row>
-    <row r="22" spans="1:14" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="72" t="s">
-        <v>2</v>
-      </c>
-      <c r="B22" s="39"/>
-      <c r="C22" s="40"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="40"/>
-      <c r="F22" s="40"/>
-      <c r="G22" s="40"/>
-      <c r="H22" s="41"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="68"/>
-      <c r="K22" s="73"/>
-      <c r="L22" s="68"/>
-      <c r="M22" s="73"/>
-      <c r="N22" s="68"/>
-    </row>
-    <row r="23" spans="1:14" ht="22.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="72"/>
-      <c r="B23" s="42"/>
-      <c r="C23" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="D23" s="44"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="46" t="s">
+      <c r="C27" s="46"/>
+      <c r="D27" s="47"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="G23" s="47"/>
-      <c r="H23" s="48"/>
-      <c r="J23" s="68"/>
-      <c r="K23" s="73"/>
-      <c r="L23" s="68"/>
-      <c r="M23" s="73"/>
-      <c r="N23" s="68"/>
-    </row>
-    <row r="24" spans="1:14" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="72"/>
-      <c r="B24" s="42"/>
-      <c r="C24" s="49"/>
-      <c r="D24" s="50"/>
-      <c r="E24" s="45"/>
-      <c r="F24" s="51"/>
-      <c r="G24" s="52"/>
-      <c r="H24" s="48"/>
-      <c r="J24" s="68"/>
-      <c r="K24" s="73"/>
-      <c r="L24" s="68"/>
-      <c r="M24" s="73"/>
-      <c r="N24" s="68"/>
-    </row>
-    <row r="25" spans="1:14" ht="9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="72"/>
-      <c r="B25" s="53"/>
-      <c r="C25" s="54"/>
-      <c r="D25" s="54"/>
-      <c r="E25" s="55"/>
-      <c r="F25" s="56"/>
-      <c r="G25" s="56"/>
-      <c r="H25" s="57"/>
-      <c r="J25" s="69"/>
-      <c r="K25" s="73"/>
-      <c r="L25" s="69"/>
-      <c r="M25" s="73"/>
-      <c r="N25" s="69"/>
-    </row>
-    <row r="26" spans="1:14" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="20"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
-      <c r="J26" s="20"/>
-      <c r="L26" s="20"/>
-      <c r="N26" s="20"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B27" s="58" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" s="59"/>
-      <c r="D27" s="60"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="58" t="s">
-        <v>15</v>
-      </c>
-      <c r="G27" s="59"/>
-      <c r="H27" s="60"/>
-      <c r="J27" s="20"/>
-      <c r="L27" s="20"/>
-      <c r="N27" s="20"/>
+      <c r="G27" s="46"/>
+      <c r="H27" s="47"/>
+      <c r="J27" s="11"/>
+      <c r="L27" s="11"/>
+      <c r="N27" s="11"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B28" s="61"/>
-      <c r="C28" s="62"/>
-      <c r="D28" s="63"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="61"/>
-      <c r="G28" s="62"/>
-      <c r="H28" s="63"/>
-      <c r="J28" s="20"/>
-      <c r="L28" s="20"/>
-      <c r="N28" s="20"/>
+      <c r="B28" s="48"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="48"/>
+      <c r="G28" s="49"/>
+      <c r="H28" s="50"/>
+      <c r="J28" s="11"/>
+      <c r="L28" s="11"/>
+      <c r="N28" s="11"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B29" s="61"/>
-      <c r="C29" s="62"/>
-      <c r="D29" s="63"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="61"/>
-      <c r="G29" s="62"/>
-      <c r="H29" s="63"/>
-      <c r="J29" s="20"/>
-      <c r="L29" s="20"/>
-      <c r="N29" s="20"/>
+      <c r="B29" s="48"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="50"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="48"/>
+      <c r="G29" s="49"/>
+      <c r="H29" s="50"/>
+      <c r="J29" s="11"/>
+      <c r="L29" s="11"/>
+      <c r="N29" s="11"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B30" s="61"/>
-      <c r="C30" s="62"/>
-      <c r="D30" s="63"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="61"/>
-      <c r="G30" s="62"/>
-      <c r="H30" s="63"/>
-      <c r="J30" s="20"/>
-      <c r="L30" s="20"/>
-      <c r="N30" s="20"/>
+      <c r="B30" s="48"/>
+      <c r="C30" s="49"/>
+      <c r="D30" s="50"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="48"/>
+      <c r="G30" s="49"/>
+      <c r="H30" s="50"/>
+      <c r="J30" s="11"/>
+      <c r="L30" s="11"/>
+      <c r="N30" s="11"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B31" s="61"/>
-      <c r="C31" s="62"/>
-      <c r="D31" s="63"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="61"/>
-      <c r="G31" s="62"/>
-      <c r="H31" s="63"/>
-      <c r="J31" s="20"/>
-      <c r="L31" s="20"/>
-      <c r="N31" s="20"/>
+      <c r="B31" s="48"/>
+      <c r="C31" s="49"/>
+      <c r="D31" s="50"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="48"/>
+      <c r="G31" s="49"/>
+      <c r="H31" s="50"/>
+      <c r="J31" s="11"/>
+      <c r="L31" s="11"/>
+      <c r="N31" s="11"/>
     </row>
     <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="64"/>
-      <c r="C32" s="65"/>
-      <c r="D32" s="66"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="64"/>
-      <c r="G32" s="65"/>
-      <c r="H32" s="66"/>
-      <c r="J32" s="20"/>
-      <c r="L32" s="20"/>
-      <c r="N32" s="20"/>
+      <c r="B32" s="51"/>
+      <c r="C32" s="52"/>
+      <c r="D32" s="53"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="51"/>
+      <c r="G32" s="52"/>
+      <c r="H32" s="53"/>
+      <c r="J32" s="11"/>
+      <c r="L32" s="11"/>
+      <c r="N32" s="11"/>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B33" s="20"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="20"/>
-      <c r="G33" s="20"/>
-      <c r="H33" s="20"/>
-      <c r="J33" s="20"/>
-      <c r="L33" s="20"/>
-      <c r="N33" s="20"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="J33" s="11"/>
+      <c r="L33" s="11"/>
+      <c r="N33" s="11"/>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B34" s="20"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="20"/>
-      <c r="J34" s="20"/>
-      <c r="L34" s="20"/>
-      <c r="N34" s="20"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="J34" s="11"/>
+      <c r="L34" s="11"/>
+      <c r="N34" s="11"/>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B35" s="20"/>
-      <c r="C35" s="20"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="20"/>
-      <c r="G35" s="20"/>
-      <c r="H35" s="20"/>
-      <c r="J35" s="20"/>
-      <c r="L35" s="20"/>
-      <c r="N35" s="20"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+      <c r="J35" s="11"/>
+      <c r="L35" s="11"/>
+      <c r="N35" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="J9:J25"/>
-    <mergeCell ref="L9:L25"/>
-    <mergeCell ref="N9:N25"/>
-    <mergeCell ref="C23:D24"/>
-    <mergeCell ref="F23:G24"/>
-    <mergeCell ref="B27:D32"/>
-    <mergeCell ref="F27:H32"/>
-    <mergeCell ref="A9:A13"/>
-    <mergeCell ref="A15:A20"/>
-    <mergeCell ref="A22:A25"/>
     <mergeCell ref="B2:H6"/>
     <mergeCell ref="C10:G10"/>
     <mergeCell ref="C12:G12"/>
@@ -2117,6 +2108,16 @@
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="E18:E19"/>
     <mergeCell ref="G18:G19"/>
+    <mergeCell ref="B27:D32"/>
+    <mergeCell ref="F27:H32"/>
+    <mergeCell ref="A9:A13"/>
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="J9:J25"/>
+    <mergeCell ref="L9:L25"/>
+    <mergeCell ref="N9:N25"/>
+    <mergeCell ref="C23:D24"/>
+    <mergeCell ref="F23:G24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>